<commit_message>
Staff Members loader with Excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataloader.xlsx
+++ b/src/main/resources/dataloader.xlsx
@@ -7,20 +7,98 @@
     <workbookView xWindow="480" yWindow="144" windowWidth="22116" windowHeight="8760"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="staff" sheetId="1" r:id="rId1"/>
+    <sheet name="conf" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>HasCar</t>
+  </si>
+  <si>
+    <t>CorporateEmail</t>
+  </si>
+  <si>
+    <t>CommunicationLanguage</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>john.doe@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>jane.white@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Dupont</t>
+  </si>
+  <si>
+    <t>jean.dupont@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Pieters</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -43,13 +121,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,36 +430,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please choose &quot;yes&quot; or &quot;no&quot;" promptTitle="Please choose &quot;yes&quot; or &quot;no&quot;">
+          <x14:formula1>
+            <xm:f>conf!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C3648</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please choose FR NL or EN" promptTitle="Please choose FR NL or EN">
+          <x14:formula1>
+            <xm:f>conf!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E2340</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added method to retrieve staff members without car
</commit_message>
<xml_diff>
--- a/src/main/resources/dataloader.xlsx
+++ b/src/main/resources/dataloader.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>FirstName</t>
   </si>
@@ -81,6 +81,27 @@
   </si>
   <si>
     <t>Pieters</t>
+  </si>
+  <si>
+    <t>jan.pieters@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Dubois</t>
+  </si>
+  <si>
+    <t>paul.dubois@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Rakia</t>
+  </si>
+  <si>
+    <t>Madour</t>
+  </si>
+  <si>
+    <t>rakia.madour@soprasteria.com</t>
   </si>
 </sst>
 </file>
@@ -430,11 +451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,12 +539,58 @@
       <c r="B5" t="s">
         <v>21</v>
       </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Staff member update (hasCar) is written to Excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataloader.xlsx
+++ b/src/main/resources/dataloader.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>FirstName</t>
   </si>
@@ -102,12 +102,109 @@
   </si>
   <si>
     <t>rakia.madour@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Giselle</t>
+  </si>
+  <si>
+    <t>Daoust</t>
+  </si>
+  <si>
+    <t>giselle.daoust@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Saskia</t>
+  </si>
+  <si>
+    <t>Dewit</t>
+  </si>
+  <si>
+    <t>saskia.dewit@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Hakim</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>hakim.patel@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Jos</t>
+  </si>
+  <si>
+    <t>Van Brugge</t>
+  </si>
+  <si>
+    <t>jos.vanbrugge@soprasteria.com</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Dumont</t>
+  </si>
+  <si>
+    <t>pierre.dumont@soprasteria.com</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Florence</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>florence.mary@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>erik.pieters@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Raul</t>
+  </si>
+  <si>
+    <t>Cerveza</t>
+  </si>
+  <si>
+    <t>raul.cerveza@soprasteria.com</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Calvez</t>
+  </si>
+  <si>
+    <t>antonio.calvez@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Lola</t>
+  </si>
+  <si>
+    <t>Petersen</t>
+  </si>
+  <si>
+    <t>lola.petersen@soprasteria.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,17 +548,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -523,7 +620,7 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -581,6 +678,176 @@
       </c>
       <c r="E7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -591,6 +858,16 @@
     <hyperlink ref="D5" r:id="rId4"/>
     <hyperlink ref="D6" r:id="rId5"/>
     <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Fixed setCarOfStaffMember in Staff Member service returning car instead of staff member
</commit_message>
<xml_diff>
--- a/src/main/resources/dataloader.xlsx
+++ b/src/main/resources/dataloader.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="161">
   <si>
     <t>FirstName</t>
   </si>
@@ -198,13 +198,312 @@
   </si>
   <si>
     <t>lola.petersen@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Pol</t>
+  </si>
+  <si>
+    <t>Bockman</t>
+  </si>
+  <si>
+    <t>pol.bockmand@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Lila</t>
+  </si>
+  <si>
+    <t>Bruin</t>
+  </si>
+  <si>
+    <t>lila.bruin@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>michael.scott@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Dujardin</t>
+  </si>
+  <si>
+    <t>jean.dujardin@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Lorelei</t>
+  </si>
+  <si>
+    <t>Gilmore</t>
+  </si>
+  <si>
+    <t>lorelei.gilmore@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Justine</t>
+  </si>
+  <si>
+    <t>Haoui</t>
+  </si>
+  <si>
+    <t>justine.haoui@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Yuth</t>
+  </si>
+  <si>
+    <t>Panpin</t>
+  </si>
+  <si>
+    <t>yuth.panpin@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Jambon</t>
+  </si>
+  <si>
+    <t>mike.jambon@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Elliott</t>
+  </si>
+  <si>
+    <t>Toussaint</t>
+  </si>
+  <si>
+    <t>elliott.toussaint@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Gerard</t>
+  </si>
+  <si>
+    <t>De Rivia</t>
+  </si>
+  <si>
+    <t>gerard.derivia@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>de Vengerberg</t>
+  </si>
+  <si>
+    <t>jennifer.deVengerberg@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Anya</t>
+  </si>
+  <si>
+    <t>Chalotra</t>
+  </si>
+  <si>
+    <t>anya.chalotra@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Andrzej</t>
+  </si>
+  <si>
+    <t>Sapkowski</t>
+  </si>
+  <si>
+    <t>andrzej.Sapkowski@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Morty</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>morty.sanchez@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Rick</t>
+  </si>
+  <si>
+    <t>rick.sanchez@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Kira</t>
+  </si>
+  <si>
+    <t>Yagami</t>
+  </si>
+  <si>
+    <t>kira.yagami@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Arnold</t>
+  </si>
+  <si>
+    <t>Truffiaut</t>
+  </si>
+  <si>
+    <t>arnold.truffiaut@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Grégory</t>
+  </si>
+  <si>
+    <t>Sturdeur</t>
+  </si>
+  <si>
+    <t>gregory.sturdeur@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Tchaikovsky</t>
+  </si>
+  <si>
+    <t>andy.tchaikovsky@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Eddy</t>
+  </si>
+  <si>
+    <t>Hatcheur</t>
+  </si>
+  <si>
+    <t>eddy.hatcheur@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Spitz</t>
+  </si>
+  <si>
+    <t>andrew.spitz@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>andrea.yellow@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Goedman</t>
+  </si>
+  <si>
+    <t>hans.goedman@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Elise</t>
+  </si>
+  <si>
+    <t>Tatcher</t>
+  </si>
+  <si>
+    <t>elise.tatcher@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Maggy</t>
+  </si>
+  <si>
+    <t>Van Rond</t>
+  </si>
+  <si>
+    <t>maggy.vanrond@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Else</t>
+  </si>
+  <si>
+    <t>Cintra</t>
+  </si>
+  <si>
+    <t>else.cintra@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Stout</t>
+  </si>
+  <si>
+    <t>eddy.stout@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Gevadra</t>
+  </si>
+  <si>
+    <t>anna.gevadra@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Ilse</t>
+  </si>
+  <si>
+    <t>De Kooi</t>
+  </si>
+  <si>
+    <t>ilse.dekooi@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Blauw</t>
+  </si>
+  <si>
+    <t>erik.blauw@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Turdui</t>
+  </si>
+  <si>
+    <t>michael.turdui@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Toubeaux</t>
+  </si>
+  <si>
+    <t>scott.toubeaux@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Edwin</t>
+  </si>
+  <si>
+    <t>Derige</t>
+  </si>
+  <si>
+    <t>edwin.derige@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Elvis</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>elvis.alpha@soprasteria.com</t>
+  </si>
+  <si>
+    <t>Henriette</t>
+  </si>
+  <si>
+    <t>henriette.goedman@soprasteria.com</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>jean.dupont2@soprasteria.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,17 +847,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="56.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="4" max="4" width="56" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -847,6 +1146,618 @@
         <v>60</v>
       </c>
       <c r="E17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" t="s">
+        <v>159</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" t="s">
+        <v>159</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" t="s">
         <v>45</v>
       </c>
     </row>
@@ -868,6 +1779,42 @@
     <hyperlink ref="D15" r:id="rId14"/>
     <hyperlink ref="D16" r:id="rId15"/>
     <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
+    <hyperlink ref="D46" r:id="rId45"/>
+    <hyperlink ref="D47" r:id="rId46"/>
+    <hyperlink ref="D48" r:id="rId47"/>
+    <hyperlink ref="D49" r:id="rId48"/>
+    <hyperlink ref="D50" r:id="rId49"/>
+    <hyperlink ref="D51" r:id="rId50"/>
+    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D53" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>